<commit_message>
Correction erreur slice 79248e6ff8d6accb5a4f63af4ba0f723c9173176
</commit_message>
<xml_diff>
--- a/maj-sp/ig/StructureDefinition-oncofair-medicationadministration-element.xlsx
+++ b/maj-sp/ig/StructureDefinition-oncofair-medicationadministration-element.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-17T13:59:50+00:00</t>
+    <t>2025-01-17T15:20:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -717,7 +717,7 @@
     <t>http://hl7.org/fhir/ValueSet/medication-admin-location</t>
   </si>
   <si>
-    <t xml:space="preserve">value:system}
+    <t xml:space="preserve">value:coding.system}
 </t>
   </si>
   <si>

</xml_diff>